<commit_message>
Estetização simples da planilha
</commit_message>
<xml_diff>
--- a/data/processed_data/Meganium_Salas_Data.xlsx
+++ b/data/processed_data/Meganium_Salas_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACER\Desktop\BootCamp Prompt de IA Microsoft\dataset-gamesshop\data\processed_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE752141-B0F5-42C4-9707-FB5EC42BB5FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DAC2F94-CEF9-4A8B-ACFC-EE4091FDCF69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1B850798-B399-499D-BFE3-763D79448148}"/>
   </bookViews>
@@ -873,7 +873,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -881,18 +881,52 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCE3C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right/>
       <top/>
       <bottom/>
@@ -902,9 +936,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1239,2714 +1277,2722 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B36C1513-D75A-4A02-8891-8819B21FF9A5}">
-  <dimension ref="A1:N61"/>
+  <dimension ref="A1:N62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.77734375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" style="2"/>
+    <col min="6" max="6" width="9.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="36.33203125" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="5">
         <v>45538</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="2">
         <v>2</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="2">
         <v>90</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="2">
         <v>180</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="K2" s="1">
+      <c r="K2" s="5">
         <v>27322</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M2" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="N2" t="s">
+      <c r="N2" s="4" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="5">
         <v>45581</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="2">
         <v>1</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="2">
         <v>70</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="2">
         <v>70</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="K3" s="1">
+      <c r="K3" s="5">
         <v>33419</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L3" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="M3" t="s">
+      <c r="M3" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="N3" t="s">
+      <c r="N3" s="4" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="5">
         <v>45567</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="2">
         <v>4</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="2">
         <v>80</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="2">
         <v>320</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="K4" s="1">
+      <c r="K4" s="5">
         <v>28020</v>
       </c>
-      <c r="L4" t="s">
+      <c r="L4" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="M4" t="s">
+      <c r="M4" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="N4" t="s">
+      <c r="N4" s="4" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="5">
         <v>45514</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="2">
         <v>4</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="2">
         <v>90</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="2">
         <v>360</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="K5" s="1">
+      <c r="K5" s="5">
         <v>36852</v>
       </c>
-      <c r="L5" t="s">
+      <c r="L5" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="M5" t="s">
+      <c r="M5" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="N5" t="s">
+      <c r="N5" s="4" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="5">
         <v>45430</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="2">
         <v>5</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="2">
         <v>100</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="2">
         <v>500</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J6" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="K6" s="1">
+      <c r="K6" s="5">
         <v>31554</v>
       </c>
-      <c r="L6" t="s">
+      <c r="L6" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="M6" t="s">
+      <c r="M6" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="N6" t="s">
+      <c r="N6" s="4" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="A7" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="5">
         <v>45564</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="2">
         <v>1</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="2">
         <v>80</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="2">
         <v>80</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I7" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J7" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="K7" s="1">
+      <c r="K7" s="5">
         <v>31759</v>
       </c>
-      <c r="L7" t="s">
+      <c r="L7" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="M7" t="s">
+      <c r="M7" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="N7" t="s">
+      <c r="N7" s="4" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="A8" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="5">
         <v>45525</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="2">
         <v>4</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="2">
         <v>70</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="2">
         <v>280</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I8" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J8" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="K8" s="1">
+      <c r="K8" s="5">
         <v>26004</v>
       </c>
-      <c r="L8" t="s">
+      <c r="L8" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="M8" t="s">
+      <c r="M8" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="N8" t="s">
+      <c r="N8" s="4" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="A9" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="5">
         <v>45546</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="2">
         <v>2</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="2">
         <v>80</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="2">
         <v>160</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I9" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J9" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="K9" s="1">
+      <c r="K9" s="5">
         <v>32351</v>
       </c>
-      <c r="L9" t="s">
+      <c r="L9" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="M9" t="s">
+      <c r="M9" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="N9" t="s">
+      <c r="N9" s="4" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="A10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="5">
         <v>45557</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="2">
         <v>1</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="2">
         <v>100</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="2">
         <v>100</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H10" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I10" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="J10" t="s">
+      <c r="J10" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="K10" s="1">
+      <c r="K10" s="5">
         <v>28723</v>
       </c>
-      <c r="L10" t="s">
+      <c r="L10" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="M10" t="s">
+      <c r="M10" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="N10" t="s">
+      <c r="N10" s="4" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="A11" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="5">
         <v>45553</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="2">
         <v>4</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="2">
         <v>70</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="2">
         <v>280</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H11" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="I11" t="s">
+      <c r="I11" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="J11" t="s">
+      <c r="J11" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="K11" s="1">
+      <c r="K11" s="5">
         <v>34003</v>
       </c>
-      <c r="L11" t="s">
+      <c r="L11" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="M11" t="s">
+      <c r="M11" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="N11" t="s">
+      <c r="N11" s="4" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="A12" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="5">
         <v>45512</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="2">
         <v>1</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="2">
         <v>80</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="2">
         <v>80</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H12" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="I12" t="s">
+      <c r="I12" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="J12" t="s">
+      <c r="J12" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="K12" s="1">
+      <c r="K12" s="5">
         <v>29590</v>
       </c>
-      <c r="L12" t="s">
+      <c r="L12" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="M12" t="s">
+      <c r="M12" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="N12" t="s">
+      <c r="N12" s="4" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="A13" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13" s="5">
         <v>45581</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="2">
         <v>4</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="2">
         <v>90</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="2">
         <v>360</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G13" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="H13" t="s">
+      <c r="H13" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="I13" t="s">
+      <c r="I13" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="J13" t="s">
+      <c r="J13" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="K13" s="1">
+      <c r="K13" s="5">
         <v>27065</v>
       </c>
-      <c r="L13" t="s">
+      <c r="L13" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="M13" t="s">
+      <c r="M13" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="N13" t="s">
+      <c r="N13" s="4" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14" s="5">
         <v>45543</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="2">
         <v>4</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="2">
         <v>100</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="2">
         <v>400</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G14" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="H14" t="s">
+      <c r="H14" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="I14" t="s">
+      <c r="I14" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="J14" t="s">
+      <c r="J14" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="K14" s="1">
+      <c r="K14" s="5">
         <v>26089</v>
       </c>
-      <c r="L14" t="s">
+      <c r="L14" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="M14" t="s">
+      <c r="M14" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="N14" t="s">
+      <c r="N14" s="4" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="A15" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15" s="5">
         <v>45520</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="2">
         <v>3</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="2">
         <v>110</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="2">
         <v>330</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G15" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="H15" t="s">
+      <c r="H15" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="I15" t="s">
+      <c r="I15" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="J15" t="s">
+      <c r="J15" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="K15" s="1">
+      <c r="K15" s="5">
         <v>28475</v>
       </c>
-      <c r="L15" t="s">
+      <c r="L15" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="M15" t="s">
+      <c r="M15" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="N15" t="s">
+      <c r="N15" s="4" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="A16" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16" s="5">
         <v>45465</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="2">
         <v>4</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="2">
         <v>80</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="2">
         <v>320</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G16" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H16" t="s">
+      <c r="H16" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="I16" t="s">
+      <c r="I16" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="J16" t="s">
+      <c r="J16" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="K16" s="1">
+      <c r="K16" s="5">
         <v>24289</v>
       </c>
-      <c r="L16" t="s">
+      <c r="L16" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="M16" t="s">
+      <c r="M16" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="N16" t="s">
+      <c r="N16" s="4" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="A17" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17" s="5">
         <v>45511</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="2">
         <v>3</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="2">
         <v>110</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="2">
         <v>330</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G17" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H17" t="s">
+      <c r="H17" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="I17" t="s">
+      <c r="I17" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="J17" t="s">
+      <c r="J17" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="K17" s="1">
+      <c r="K17" s="5">
         <v>31393</v>
       </c>
-      <c r="L17" t="s">
+      <c r="L17" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="M17" t="s">
+      <c r="M17" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="N17" t="s">
+      <c r="N17" s="4" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="A18" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18" s="5">
         <v>45475</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="2">
         <v>3</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="2">
         <v>110</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="2">
         <v>330</v>
       </c>
-      <c r="G18" t="s">
+      <c r="G18" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="H18" t="s">
+      <c r="H18" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="I18" t="s">
+      <c r="I18" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="J18" t="s">
+      <c r="J18" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="K18" s="1">
+      <c r="K18" s="5">
         <v>32598</v>
       </c>
-      <c r="L18" t="s">
+      <c r="L18" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="M18" t="s">
+      <c r="M18" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="N18" t="s">
+      <c r="N18" s="4" t="s">
         <v>264</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="A19" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C19" s="5">
         <v>45496</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="2">
         <v>3</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="2">
         <v>90</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="2">
         <v>270</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G19" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H19" t="s">
+      <c r="H19" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="I19" t="s">
+      <c r="I19" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="J19" t="s">
+      <c r="J19" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="K19" s="1">
+      <c r="K19" s="5">
         <v>38381</v>
       </c>
-      <c r="L19" t="s">
+      <c r="L19" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="M19" t="s">
+      <c r="M19" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="N19" t="s">
+      <c r="N19" s="4" t="s">
         <v>268</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+      <c r="A20" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C20" s="5">
         <v>45572</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="2">
         <v>4</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="2">
         <v>70</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="2">
         <v>280</v>
       </c>
-      <c r="G20" t="s">
+      <c r="G20" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="H20" t="s">
+      <c r="H20" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="I20" t="s">
+      <c r="I20" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="J20" t="s">
+      <c r="J20" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="K20" s="1">
+      <c r="K20" s="5">
         <v>32146</v>
       </c>
-      <c r="L20" t="s">
+      <c r="L20" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="M20" t="s">
+      <c r="M20" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="N20" t="s">
+      <c r="N20" s="4" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+      <c r="A21" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C21" s="1">
+      <c r="C21" s="5">
         <v>45525</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="2">
         <v>1</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="2">
         <v>90</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="2">
         <v>90</v>
       </c>
-      <c r="G21" t="s">
+      <c r="G21" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="H21" t="s">
+      <c r="H21" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="I21" t="s">
+      <c r="I21" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="J21" t="s">
+      <c r="J21" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="K21" s="1">
+      <c r="K21" s="5">
         <v>34963</v>
       </c>
-      <c r="L21" t="s">
+      <c r="L21" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="M21" t="s">
+      <c r="M21" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="N21" t="s">
+      <c r="N21" s="4" t="s">
         <v>276</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+      <c r="A22" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C22" s="1">
+      <c r="C22" s="5">
         <v>45560</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="2">
         <v>5</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="2">
         <v>100</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="2">
         <v>500</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G22" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="H22" t="s">
+      <c r="H22" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="I22" t="s">
+      <c r="I22" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="J22" t="s">
+      <c r="J22" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="K22" s="1">
+      <c r="K22" s="5">
         <v>28136</v>
       </c>
-      <c r="L22" t="s">
+      <c r="L22" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="M22" t="s">
+      <c r="M22" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="N22" t="s">
+      <c r="N22" s="4" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+      <c r="A23" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C23" s="1">
+      <c r="C23" s="5">
         <v>45524</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="2">
         <v>2</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="2">
         <v>90</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="2">
         <v>180</v>
       </c>
-      <c r="G23" t="s">
+      <c r="G23" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="H23" t="s">
+      <c r="H23" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="I23" t="s">
+      <c r="I23" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="J23" t="s">
+      <c r="J23" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="K23" s="1">
+      <c r="K23" s="5">
         <v>31155</v>
       </c>
-      <c r="L23" t="s">
+      <c r="L23" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="M23" t="s">
+      <c r="M23" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="N23" t="s">
+      <c r="N23" s="4" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+      <c r="A24" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C24" s="5">
         <v>45595</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="2">
         <v>5</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="2">
         <v>80</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="2">
         <v>400</v>
       </c>
-      <c r="G24" t="s">
+      <c r="G24" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H24" t="s">
+      <c r="H24" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="I24" t="s">
+      <c r="I24" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="J24" t="s">
+      <c r="J24" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="K24" s="1">
+      <c r="K24" s="5">
         <v>36657</v>
       </c>
-      <c r="L24" t="s">
+      <c r="L24" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="M24" t="s">
+      <c r="M24" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="N24" t="s">
+      <c r="N24" s="4" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+      <c r="A25" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C25" s="1">
+      <c r="C25" s="5">
         <v>45564</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="2">
         <v>2</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="2">
         <v>100</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="2">
         <v>200</v>
       </c>
-      <c r="G25" t="s">
+      <c r="G25" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="H25" t="s">
+      <c r="H25" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="I25" t="s">
+      <c r="I25" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="J25" t="s">
+      <c r="J25" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="K25" s="1">
+      <c r="K25" s="5">
         <v>27018</v>
       </c>
-      <c r="L25" t="s">
+      <c r="L25" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="M25" t="s">
+      <c r="M25" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="N25" t="s">
+      <c r="N25" s="4" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+      <c r="A26" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C26" s="1">
+      <c r="C26" s="5">
         <v>45546</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="2">
         <v>1</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="2">
         <v>110</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="2">
         <v>110</v>
       </c>
-      <c r="G26" t="s">
+      <c r="G26" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="H26" t="s">
+      <c r="H26" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="I26" t="s">
+      <c r="I26" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="J26" t="s">
+      <c r="J26" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="K26" s="1">
+      <c r="K26" s="5">
         <v>27899</v>
       </c>
-      <c r="L26" t="s">
+      <c r="L26" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="M26" t="s">
+      <c r="M26" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="N26" t="s">
+      <c r="N26" s="4" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+      <c r="A27" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C27" s="1">
+      <c r="C27" s="5">
         <v>45500</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="2">
         <v>3</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="2">
         <v>70</v>
       </c>
-      <c r="F27">
+      <c r="F27" s="2">
         <v>210</v>
       </c>
-      <c r="G27" t="s">
+      <c r="G27" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="H27" t="s">
+      <c r="H27" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="I27" t="s">
+      <c r="I27" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="J27" t="s">
+      <c r="J27" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="K27" s="1">
+      <c r="K27" s="5">
         <v>32090</v>
       </c>
-      <c r="L27" t="s">
+      <c r="L27" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="M27" t="s">
+      <c r="M27" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="N27" t="s">
+      <c r="N27" s="4" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+      <c r="A28" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C28" s="1">
+      <c r="C28" s="5">
         <v>45574</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="2">
         <v>5</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="2">
         <v>70</v>
       </c>
-      <c r="F28">
+      <c r="F28" s="2">
         <v>350</v>
       </c>
-      <c r="G28" t="s">
+      <c r="G28" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="H28" t="s">
+      <c r="H28" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="I28" t="s">
+      <c r="I28" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="J28" t="s">
+      <c r="J28" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="K28" s="1">
+      <c r="K28" s="5">
         <v>38606</v>
       </c>
-      <c r="L28" t="s">
+      <c r="L28" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="M28" t="s">
+      <c r="M28" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="N28" t="s">
+      <c r="N28" s="4" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+      <c r="A29" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C29" s="1">
+      <c r="C29" s="5">
         <v>45549</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="2">
         <v>5</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="2">
         <v>90</v>
       </c>
-      <c r="F29">
+      <c r="F29" s="2">
         <v>450</v>
       </c>
-      <c r="G29" t="s">
+      <c r="G29" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H29" t="s">
+      <c r="H29" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="I29" t="s">
+      <c r="I29" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="J29" t="s">
+      <c r="J29" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="K29" s="1">
+      <c r="K29" s="5">
         <v>29892</v>
       </c>
-      <c r="L29" t="s">
+      <c r="L29" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="M29" t="s">
+      <c r="M29" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="N29" t="s">
+      <c r="N29" s="4" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
+      <c r="A30" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C30" s="1">
+      <c r="C30" s="5">
         <v>45529</v>
       </c>
-      <c r="D30">
+      <c r="D30" s="2">
         <v>5</v>
       </c>
-      <c r="E30">
+      <c r="E30" s="2">
         <v>110</v>
       </c>
-      <c r="F30">
+      <c r="F30" s="2">
         <v>550</v>
       </c>
-      <c r="G30" t="s">
+      <c r="G30" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="H30" t="s">
+      <c r="H30" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="I30" t="s">
+      <c r="I30" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="J30" t="s">
+      <c r="J30" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="K30" s="1">
+      <c r="K30" s="5">
         <v>26295</v>
       </c>
-      <c r="L30" t="s">
+      <c r="L30" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="M30" t="s">
+      <c r="M30" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="N30" t="s">
+      <c r="N30" s="4" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
+      <c r="A31" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C31" s="1">
+      <c r="C31" s="5">
         <v>45450</v>
       </c>
-      <c r="D31">
+      <c r="D31" s="2">
         <v>5</v>
       </c>
-      <c r="E31">
+      <c r="E31" s="2">
         <v>100</v>
       </c>
-      <c r="F31">
+      <c r="F31" s="2">
         <v>500</v>
       </c>
-      <c r="G31" t="s">
+      <c r="G31" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H31" t="s">
+      <c r="H31" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="I31" t="s">
+      <c r="I31" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="J31" t="s">
+      <c r="J31" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="K31" s="1">
+      <c r="K31" s="5">
         <v>28332</v>
       </c>
-      <c r="L31" t="s">
+      <c r="L31" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="M31" t="s">
+      <c r="M31" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="N31" t="s">
+      <c r="N31" s="4" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
+      <c r="A32" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C32" s="1">
+      <c r="C32" s="5">
         <v>45480</v>
       </c>
-      <c r="D32">
+      <c r="D32" s="2">
         <v>1</v>
       </c>
-      <c r="E32">
+      <c r="E32" s="2">
         <v>100</v>
       </c>
-      <c r="F32">
+      <c r="F32" s="2">
         <v>100</v>
       </c>
-      <c r="G32" t="s">
+      <c r="G32" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="H32" t="s">
+      <c r="H32" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="I32" t="s">
+      <c r="I32" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="J32" t="s">
+      <c r="J32" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="K32" s="1">
+      <c r="K32" s="5">
         <v>34761</v>
       </c>
-      <c r="L32" t="s">
+      <c r="L32" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="M32" t="s">
+      <c r="M32" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="N32" t="s">
+      <c r="N32" s="4" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
+      <c r="A33" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C33" s="1">
+      <c r="C33" s="5">
         <v>45585</v>
       </c>
-      <c r="D33">
+      <c r="D33" s="2">
         <v>2</v>
       </c>
-      <c r="E33">
+      <c r="E33" s="2">
         <v>70</v>
       </c>
-      <c r="F33">
+      <c r="F33" s="2">
         <v>140</v>
       </c>
-      <c r="G33" t="s">
+      <c r="G33" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="H33" t="s">
+      <c r="H33" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="I33" t="s">
+      <c r="I33" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="J33" t="s">
+      <c r="J33" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="K33" s="1">
+      <c r="K33" s="5">
         <v>29466</v>
       </c>
-      <c r="L33" t="s">
+      <c r="L33" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="M33" t="s">
+      <c r="M33" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="N33" t="s">
+      <c r="N33" s="4" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
+      <c r="A34" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C34" s="1">
+      <c r="C34" s="5">
         <v>45440</v>
       </c>
-      <c r="D34">
+      <c r="D34" s="2">
         <v>3</v>
       </c>
-      <c r="E34">
+      <c r="E34" s="2">
         <v>80</v>
       </c>
-      <c r="F34">
+      <c r="F34" s="2">
         <v>240</v>
       </c>
-      <c r="G34" t="s">
+      <c r="G34" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="H34" t="s">
+      <c r="H34" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="I34" t="s">
+      <c r="I34" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="J34" t="s">
+      <c r="J34" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="K34" s="1">
+      <c r="K34" s="5">
         <v>27099</v>
       </c>
-      <c r="L34" t="s">
+      <c r="L34" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="M34" t="s">
+      <c r="M34" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="N34" t="s">
+      <c r="N34" s="4" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
+      <c r="A35" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C35" s="1">
+      <c r="C35" s="5">
         <v>45592</v>
       </c>
-      <c r="D35">
+      <c r="D35" s="2">
         <v>3</v>
       </c>
-      <c r="E35">
+      <c r="E35" s="2">
         <v>70</v>
       </c>
-      <c r="F35">
+      <c r="F35" s="2">
         <v>210</v>
       </c>
-      <c r="G35" t="s">
+      <c r="G35" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="H35" t="s">
+      <c r="H35" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="I35" t="s">
+      <c r="I35" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="J35" t="s">
+      <c r="J35" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="K35" s="1">
+      <c r="K35" s="5">
         <v>35513</v>
       </c>
-      <c r="L35" t="s">
+      <c r="L35" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="M35" t="s">
+      <c r="M35" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="N35" t="s">
+      <c r="N35" s="4" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
+      <c r="A36" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C36" s="1">
+      <c r="C36" s="5">
         <v>45467</v>
       </c>
-      <c r="D36">
+      <c r="D36" s="2">
         <v>4</v>
       </c>
-      <c r="E36">
+      <c r="E36" s="2">
         <v>80</v>
       </c>
-      <c r="F36">
+      <c r="F36" s="2">
         <v>320</v>
       </c>
-      <c r="G36" t="s">
+      <c r="G36" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="H36" t="s">
+      <c r="H36" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="I36" t="s">
+      <c r="I36" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="J36" t="s">
+      <c r="J36" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="K36" s="1">
+      <c r="K36" s="5">
         <v>24021</v>
       </c>
-      <c r="L36" t="s">
+      <c r="L36" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="M36" t="s">
+      <c r="M36" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="N36" t="s">
+      <c r="N36" s="4" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
+      <c r="A37" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C37" s="1">
+      <c r="C37" s="5">
         <v>45563</v>
       </c>
-      <c r="D37">
+      <c r="D37" s="2">
         <v>2</v>
       </c>
-      <c r="E37">
+      <c r="E37" s="2">
         <v>80</v>
       </c>
-      <c r="F37">
+      <c r="F37" s="2">
         <v>160</v>
       </c>
-      <c r="G37" t="s">
+      <c r="G37" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H37" t="s">
+      <c r="H37" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="I37" t="s">
+      <c r="I37" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="J37" t="s">
+      <c r="J37" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="K37" s="1">
+      <c r="K37" s="5">
         <v>35903</v>
       </c>
-      <c r="L37" t="s">
+      <c r="L37" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="M37" t="s">
+      <c r="M37" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="N37" t="s">
+      <c r="N37" s="4" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
+      <c r="A38" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C38" s="1">
+      <c r="C38" s="5">
         <v>45522</v>
       </c>
-      <c r="D38">
+      <c r="D38" s="2">
         <v>1</v>
       </c>
-      <c r="E38">
+      <c r="E38" s="2">
         <v>100</v>
       </c>
-      <c r="F38">
+      <c r="F38" s="2">
         <v>100</v>
       </c>
-      <c r="G38" t="s">
+      <c r="G38" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="H38" t="s">
+      <c r="H38" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="I38" t="s">
+      <c r="I38" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="J38" t="s">
+      <c r="J38" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="K38" s="1">
+      <c r="K38" s="5">
         <v>30079</v>
       </c>
-      <c r="L38" t="s">
+      <c r="L38" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="M38" t="s">
+      <c r="M38" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="N38" t="s">
+      <c r="N38" s="4" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
+      <c r="A39" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C39" s="1">
+      <c r="C39" s="5">
         <v>45481</v>
       </c>
-      <c r="D39">
+      <c r="D39" s="2">
         <v>4</v>
       </c>
-      <c r="E39">
+      <c r="E39" s="2">
         <v>80</v>
       </c>
-      <c r="F39">
+      <c r="F39" s="2">
         <v>320</v>
       </c>
-      <c r="G39" t="s">
+      <c r="G39" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="H39" t="s">
+      <c r="H39" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="I39" t="s">
+      <c r="I39" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="J39" t="s">
+      <c r="J39" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="K39" s="1">
+      <c r="K39" s="5">
         <v>33313</v>
       </c>
-      <c r="L39" t="s">
+      <c r="L39" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="M39" t="s">
+      <c r="M39" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="N39" t="s">
+      <c r="N39" s="4" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
+      <c r="A40" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C40" s="1">
+      <c r="C40" s="5">
         <v>45567</v>
       </c>
-      <c r="D40">
+      <c r="D40" s="2">
         <v>2</v>
       </c>
-      <c r="E40">
+      <c r="E40" s="2">
         <v>110</v>
       </c>
-      <c r="F40">
+      <c r="F40" s="2">
         <v>220</v>
       </c>
-      <c r="G40" t="s">
+      <c r="G40" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="H40" t="s">
+      <c r="H40" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="I40" t="s">
+      <c r="I40" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="J40" t="s">
+      <c r="J40" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="K40" s="1">
+      <c r="K40" s="5">
         <v>29656</v>
       </c>
-      <c r="L40" t="s">
+      <c r="L40" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="M40" t="s">
+      <c r="M40" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="N40" t="s">
+      <c r="N40" s="4" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
+      <c r="A41" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C41" s="1">
+      <c r="C41" s="5">
         <v>45592</v>
       </c>
-      <c r="D41">
+      <c r="D41" s="2">
         <v>4</v>
       </c>
-      <c r="E41">
+      <c r="E41" s="2">
         <v>90</v>
       </c>
-      <c r="F41">
+      <c r="F41" s="2">
         <v>360</v>
       </c>
-      <c r="G41" t="s">
+      <c r="G41" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="H41" t="s">
+      <c r="H41" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="I41" t="s">
+      <c r="I41" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="J41" t="s">
+      <c r="J41" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="K41" s="1">
+      <c r="K41" s="5">
         <v>26546</v>
       </c>
-      <c r="L41" t="s">
+      <c r="L41" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="M41" t="s">
+      <c r="M41" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="N41" t="s">
+      <c r="N41" s="4" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
+      <c r="A42" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C42" s="1">
+      <c r="C42" s="5">
         <v>45535</v>
       </c>
-      <c r="D42">
+      <c r="D42" s="2">
         <v>4</v>
       </c>
-      <c r="E42">
+      <c r="E42" s="2">
         <v>100</v>
       </c>
-      <c r="F42">
+      <c r="F42" s="2">
         <v>400</v>
       </c>
-      <c r="G42" t="s">
+      <c r="G42" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H42" t="s">
+      <c r="H42" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I42" t="s">
+      <c r="I42" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J42" t="s">
+      <c r="J42" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="K42" s="1">
+      <c r="K42" s="5">
         <v>38668</v>
       </c>
-      <c r="L42" t="s">
+      <c r="L42" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="M42" t="s">
+      <c r="M42" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="N42" t="s">
+      <c r="N42" s="4" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
+      <c r="A43" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C43" s="1">
+      <c r="C43" s="5">
         <v>45592</v>
       </c>
-      <c r="D43">
+      <c r="D43" s="2">
         <v>3</v>
       </c>
-      <c r="E43">
+      <c r="E43" s="2">
         <v>90</v>
       </c>
-      <c r="F43">
+      <c r="F43" s="2">
         <v>270</v>
       </c>
-      <c r="G43" t="s">
+      <c r="G43" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H43" t="s">
+      <c r="H43" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I43" t="s">
+      <c r="I43" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="J43" t="s">
+      <c r="J43" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="K43" s="1">
+      <c r="K43" s="5">
         <v>28271</v>
       </c>
-      <c r="L43" t="s">
+      <c r="L43" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="M43" t="s">
+      <c r="M43" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="N43" t="s">
+      <c r="N43" s="4" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
+      <c r="A44" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C44" s="1">
+      <c r="C44" s="5">
         <v>45507</v>
       </c>
-      <c r="D44">
+      <c r="D44" s="2">
         <v>1</v>
       </c>
-      <c r="E44">
+      <c r="E44" s="2">
         <v>80</v>
       </c>
-      <c r="F44">
+      <c r="F44" s="2">
         <v>80</v>
       </c>
-      <c r="G44" t="s">
+      <c r="G44" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="H44" t="s">
+      <c r="H44" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I44" t="s">
+      <c r="I44" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="J44" t="s">
+      <c r="J44" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="K44" s="1">
+      <c r="K44" s="5">
         <v>24837</v>
       </c>
-      <c r="L44" t="s">
+      <c r="L44" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="M44" t="s">
+      <c r="M44" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="N44" t="s">
+      <c r="N44" s="4" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
+      <c r="A45" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C45" s="1">
+      <c r="C45" s="5">
         <v>45545</v>
       </c>
-      <c r="D45">
+      <c r="D45" s="2">
         <v>4</v>
       </c>
-      <c r="E45">
+      <c r="E45" s="2">
         <v>110</v>
       </c>
-      <c r="F45">
+      <c r="F45" s="2">
         <v>440</v>
       </c>
-      <c r="G45" t="s">
+      <c r="G45" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="H45" t="s">
+      <c r="H45" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I45" t="s">
+      <c r="I45" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="J45" t="s">
+      <c r="J45" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="K45" s="1">
+      <c r="K45" s="5">
         <v>30837</v>
       </c>
-      <c r="L45" t="s">
+      <c r="L45" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="M45" t="s">
+      <c r="M45" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="N45" t="s">
+      <c r="N45" s="4" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
+      <c r="A46" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C46" s="1">
+      <c r="C46" s="5">
         <v>45518</v>
       </c>
-      <c r="D46">
+      <c r="D46" s="2">
         <v>5</v>
       </c>
-      <c r="E46">
+      <c r="E46" s="2">
         <v>70</v>
       </c>
-      <c r="F46">
+      <c r="F46" s="2">
         <v>350</v>
       </c>
-      <c r="G46" t="s">
+      <c r="G46" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H46" t="s">
+      <c r="H46" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I46" t="s">
+      <c r="I46" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="J46" t="s">
+      <c r="J46" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="K46" s="1">
+      <c r="K46" s="5">
         <v>32090</v>
       </c>
-      <c r="L46" t="s">
+      <c r="L46" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="M46" t="s">
+      <c r="M46" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="N46" t="s">
+      <c r="N46" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
+      <c r="A47" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C47" s="1">
+      <c r="C47" s="5">
         <v>45454</v>
       </c>
-      <c r="D47">
+      <c r="D47" s="2">
         <v>5</v>
       </c>
-      <c r="E47">
+      <c r="E47" s="2">
         <v>90</v>
       </c>
-      <c r="F47">
+      <c r="F47" s="2">
         <v>450</v>
       </c>
-      <c r="G47" t="s">
+      <c r="G47" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="H47" t="s">
+      <c r="H47" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I47" t="s">
+      <c r="I47" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="J47" t="s">
+      <c r="J47" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="K47" s="1">
+      <c r="K47" s="5">
         <v>27859</v>
       </c>
-      <c r="L47" t="s">
+      <c r="L47" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="M47" t="s">
+      <c r="M47" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="N47" t="s">
+      <c r="N47" s="4" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
+      <c r="A48" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C48" s="1">
+      <c r="C48" s="5">
         <v>45510</v>
       </c>
-      <c r="D48">
+      <c r="D48" s="2">
         <v>5</v>
       </c>
-      <c r="E48">
+      <c r="E48" s="2">
         <v>100</v>
       </c>
-      <c r="F48">
+      <c r="F48" s="2">
         <v>500</v>
       </c>
-      <c r="G48" t="s">
+      <c r="G48" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="H48" t="s">
+      <c r="H48" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I48" t="s">
+      <c r="I48" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="J48" t="s">
+      <c r="J48" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="K48" s="1">
+      <c r="K48" s="5">
         <v>26827</v>
       </c>
-      <c r="L48" t="s">
+      <c r="L48" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="M48" t="s">
+      <c r="M48" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="N48" t="s">
+      <c r="N48" s="4" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
+      <c r="A49" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C49" s="1">
+      <c r="C49" s="5">
         <v>45495</v>
       </c>
-      <c r="D49">
+      <c r="D49" s="2">
         <v>3</v>
       </c>
-      <c r="E49">
+      <c r="E49" s="2">
         <v>70</v>
       </c>
-      <c r="F49">
+      <c r="F49" s="2">
         <v>210</v>
       </c>
-      <c r="G49" t="s">
+      <c r="G49" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="H49" t="s">
+      <c r="H49" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I49" t="s">
+      <c r="I49" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="J49" t="s">
+      <c r="J49" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="K49" s="1">
+      <c r="K49" s="5">
         <v>26181</v>
       </c>
-      <c r="L49" t="s">
+      <c r="L49" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="M49" t="s">
+      <c r="M49" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="N49" t="s">
+      <c r="N49" s="4" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
+      <c r="A50" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C50" s="1">
+      <c r="C50" s="5">
         <v>45528</v>
       </c>
-      <c r="D50">
+      <c r="D50" s="2">
         <v>2</v>
       </c>
-      <c r="E50">
+      <c r="E50" s="2">
         <v>90</v>
       </c>
-      <c r="F50">
+      <c r="F50" s="2">
         <v>180</v>
       </c>
-      <c r="G50" t="s">
+      <c r="G50" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="H50" t="s">
+      <c r="H50" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I50" t="s">
+      <c r="I50" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="J50" t="s">
+      <c r="J50" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="K50" s="1">
+      <c r="K50" s="5">
         <v>32654</v>
       </c>
-      <c r="L50" t="s">
+      <c r="L50" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="M50" t="s">
+      <c r="M50" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="N50" t="s">
+      <c r="N50" s="4" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
+      <c r="A51" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B51" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C51" s="1">
+      <c r="C51" s="5">
         <v>45542</v>
       </c>
-      <c r="D51">
+      <c r="D51" s="2">
         <v>1</v>
       </c>
-      <c r="E51">
+      <c r="E51" s="2">
         <v>70</v>
       </c>
-      <c r="F51">
+      <c r="F51" s="2">
         <v>70</v>
       </c>
-      <c r="G51" t="s">
+      <c r="G51" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H51" t="s">
+      <c r="H51" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I51" t="s">
+      <c r="I51" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="J51" t="s">
+      <c r="J51" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="K51" s="1">
+      <c r="K51" s="5">
         <v>23925</v>
       </c>
-      <c r="L51" t="s">
+      <c r="L51" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="M51" t="s">
+      <c r="M51" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="N51" t="s">
+      <c r="N51" s="4" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
+      <c r="A52" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B52" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C52" s="1">
+      <c r="C52" s="5">
         <v>45496</v>
       </c>
-      <c r="D52">
+      <c r="D52" s="2">
         <v>5</v>
       </c>
-      <c r="E52">
+      <c r="E52" s="2">
         <v>110</v>
       </c>
-      <c r="F52">
+      <c r="F52" s="2">
         <v>550</v>
       </c>
-      <c r="G52" t="s">
+      <c r="G52" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H52" t="s">
+      <c r="H52" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I52" t="s">
+      <c r="I52" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="J52" t="s">
+      <c r="J52" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="K52" s="1">
+      <c r="K52" s="5">
         <v>30343</v>
       </c>
-      <c r="L52" t="s">
+      <c r="L52" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="M52" t="s">
+      <c r="M52" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="N52" t="s">
+      <c r="N52" s="4" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
+      <c r="A53" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B53" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C53" s="1">
+      <c r="C53" s="5">
         <v>45446</v>
       </c>
-      <c r="D53">
+      <c r="D53" s="2">
         <v>1</v>
       </c>
-      <c r="E53">
+      <c r="E53" s="2">
         <v>110</v>
       </c>
-      <c r="F53">
+      <c r="F53" s="2">
         <v>110</v>
       </c>
-      <c r="G53" t="s">
+      <c r="G53" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H53" t="s">
+      <c r="H53" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I53" t="s">
+      <c r="I53" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="J53" t="s">
+      <c r="J53" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="K53" s="1">
+      <c r="K53" s="5">
         <v>33348</v>
       </c>
-      <c r="L53" t="s">
+      <c r="L53" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="M53" t="s">
+      <c r="M53" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="N53" t="s">
+      <c r="N53" s="4" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
+      <c r="A54" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B54" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C54" s="1">
+      <c r="C54" s="5">
         <v>45464</v>
       </c>
-      <c r="D54">
+      <c r="D54" s="2">
         <v>1</v>
       </c>
-      <c r="E54">
+      <c r="E54" s="2">
         <v>70</v>
       </c>
-      <c r="F54">
+      <c r="F54" s="2">
         <v>70</v>
       </c>
-      <c r="G54" t="s">
+      <c r="G54" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="H54" t="s">
+      <c r="H54" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I54" t="s">
+      <c r="I54" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="J54" t="s">
+      <c r="J54" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="K54" s="1">
+      <c r="K54" s="5">
         <v>26289</v>
       </c>
-      <c r="L54" t="s">
+      <c r="L54" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="M54" t="s">
+      <c r="M54" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="N54" t="s">
+      <c r="N54" s="4" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
+      <c r="A55" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B55" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C55" s="1">
+      <c r="C55" s="5">
         <v>45555</v>
       </c>
-      <c r="D55">
+      <c r="D55" s="2">
         <v>3</v>
       </c>
-      <c r="E55">
+      <c r="E55" s="2">
         <v>100</v>
       </c>
-      <c r="F55">
+      <c r="F55" s="2">
         <v>300</v>
       </c>
-      <c r="G55" t="s">
+      <c r="G55" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H55" t="s">
+      <c r="H55" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I55" t="s">
+      <c r="I55" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="J55" t="s">
+      <c r="J55" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="K55" s="1">
+      <c r="K55" s="5">
         <v>37251</v>
       </c>
-      <c r="L55" t="s">
+      <c r="L55" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="M55" t="s">
+      <c r="M55" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="N55" t="s">
+      <c r="N55" s="4" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
+      <c r="A56" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B56" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C56" s="1">
+      <c r="C56" s="5">
         <v>45430</v>
       </c>
-      <c r="D56">
+      <c r="D56" s="2">
         <v>3</v>
       </c>
-      <c r="E56">
+      <c r="E56" s="2">
         <v>100</v>
       </c>
-      <c r="F56">
+      <c r="F56" s="2">
         <v>300</v>
       </c>
-      <c r="G56" t="s">
+      <c r="G56" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H56" t="s">
+      <c r="H56" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I56" t="s">
+      <c r="I56" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="J56" t="s">
+      <c r="J56" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="K56" s="1">
+      <c r="K56" s="5">
         <v>29431</v>
       </c>
-      <c r="L56" t="s">
+      <c r="L56" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="M56" t="s">
+      <c r="M56" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="N56" t="s">
+      <c r="N56" s="4" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
+      <c r="A57" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B57" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C57" s="1">
+      <c r="C57" s="5">
         <v>45509</v>
       </c>
-      <c r="D57">
+      <c r="D57" s="2">
         <v>1</v>
       </c>
-      <c r="E57">
+      <c r="E57" s="2">
         <v>100</v>
       </c>
-      <c r="F57">
+      <c r="F57" s="2">
         <v>100</v>
       </c>
-      <c r="G57" t="s">
+      <c r="G57" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H57" t="s">
+      <c r="H57" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I57" t="s">
+      <c r="I57" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="J57" t="s">
+      <c r="J57" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="K57" s="1">
+      <c r="K57" s="5">
         <v>28032</v>
       </c>
-      <c r="L57" t="s">
+      <c r="L57" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="M57" t="s">
+      <c r="M57" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="N57" t="s">
+      <c r="N57" s="4" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
+      <c r="A58" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B58" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C58" s="1">
+      <c r="C58" s="5">
         <v>45567</v>
       </c>
-      <c r="D58">
+      <c r="D58" s="2">
         <v>1</v>
       </c>
-      <c r="E58">
+      <c r="E58" s="2">
         <v>100</v>
       </c>
-      <c r="F58">
+      <c r="F58" s="2">
         <v>100</v>
       </c>
-      <c r="G58" t="s">
+      <c r="G58" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="H58" t="s">
+      <c r="H58" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I58" t="s">
+      <c r="I58" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="J58" t="s">
+      <c r="J58" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="K58" s="1">
+      <c r="K58" s="5">
         <v>33396</v>
       </c>
-      <c r="L58" t="s">
+      <c r="L58" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="M58" t="s">
+      <c r="M58" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="N58" t="s">
+      <c r="N58" s="4" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
+      <c r="A59" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B59" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C59" s="1">
+      <c r="C59" s="5">
         <v>45495</v>
       </c>
-      <c r="D59">
+      <c r="D59" s="2">
         <v>1</v>
       </c>
-      <c r="E59">
+      <c r="E59" s="2">
         <v>90</v>
       </c>
-      <c r="F59">
+      <c r="F59" s="2">
         <v>90</v>
       </c>
-      <c r="G59" t="s">
+      <c r="G59" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="H59" t="s">
+      <c r="H59" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I59" t="s">
+      <c r="I59" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="J59" t="s">
+      <c r="J59" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="K59" s="1">
+      <c r="K59" s="5">
         <v>29203</v>
       </c>
-      <c r="L59" t="s">
+      <c r="L59" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="M59" t="s">
+      <c r="M59" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="N59" t="s">
+      <c r="N59" s="4" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
+      <c r="A60" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B60" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C60" s="1">
+      <c r="C60" s="5">
         <v>45499</v>
       </c>
-      <c r="D60">
+      <c r="D60" s="2">
         <v>2</v>
       </c>
-      <c r="E60">
+      <c r="E60" s="2">
         <v>110</v>
       </c>
-      <c r="F60">
+      <c r="F60" s="2">
         <v>220</v>
       </c>
-      <c r="G60" t="s">
+      <c r="G60" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="H60" t="s">
+      <c r="H60" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I60" t="s">
+      <c r="I60" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="J60" t="s">
+      <c r="J60" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="K60" s="1">
+      <c r="K60" s="5">
         <v>29023</v>
       </c>
-      <c r="L60" t="s">
+      <c r="L60" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="M60" t="s">
+      <c r="M60" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="N60" t="s">
+      <c r="N60" s="4" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
+      <c r="A61" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B61" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C61" s="1">
+      <c r="C61" s="5">
         <v>45505</v>
       </c>
-      <c r="D61">
+      <c r="D61" s="2">
         <v>5</v>
       </c>
-      <c r="E61">
+      <c r="E61" s="2">
         <v>80</v>
       </c>
-      <c r="F61">
+      <c r="F61" s="2">
         <v>400</v>
       </c>
-      <c r="G61" t="s">
+      <c r="G61" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H61" t="s">
+      <c r="H61" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I61" t="s">
+      <c r="I61" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="J61" t="s">
+      <c r="J61" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="K61" s="1">
+      <c r="K61" s="5">
         <v>25357</v>
       </c>
-      <c r="L61" t="s">
+      <c r="L61" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="M61" t="s">
+      <c r="M61" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="N61" t="s">
+      <c r="N61" s="4" t="s">
         <v>114</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="M62" s="2">
+        <f>COUNTIF(M2:M61, "Canada")</f>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>